<commit_message>
sua them thi sinh (admin)/ Còn thêm 1 thí sinh
</commit_message>
<xml_diff>
--- a/ThiDieuLenh/dsThiSinh.xlsx
+++ b/ThiDieuLenh/dsThiSinh.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Số hiệu</t>
   </si>
@@ -39,16 +39,19 @@
     <t>Nguyen Tuan Nghia</t>
   </si>
   <si>
-    <t>Le Dang Quang</t>
-  </si>
-  <si>
-    <t>B12D39</t>
+    <t>49.330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyen Van Nghia </t>
+  </si>
+  <si>
+    <t>B12D48</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,12 +89,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -103,6 +109,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -151,7 +160,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -186,7 +195,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -395,23 +404,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="9.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="9.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="18" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,47 +428,56 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>49.328000000000003</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>2019</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>49.329000000000001</v>
+        <v>49.331000000000003</v>
       </c>
       <c r="B3" s="2">
         <v>2019</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
+      <c r="C3" s="2">
+        <v>2020</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2">
-        <v>3</v>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Them option them giao vien
</commit_message>
<xml_diff>
--- a/ThiDieuLenh/dsThiSinh.xlsx
+++ b/ThiDieuLenh/dsThiSinh.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Số hiệu</t>
   </si>
@@ -36,16 +36,19 @@
     <t>B12D49</t>
   </si>
   <si>
-    <t>Nguyen Tuan Nghia</t>
-  </si>
-  <si>
-    <t>49.330</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyen Van Nghia </t>
-  </si>
-  <si>
-    <t>B12D48</t>
+    <t>49.323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bui Quang Tuan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyen Anh Tuan </t>
+  </si>
+  <si>
+    <t>Nguyen Thi Lam Vien</t>
+  </si>
+  <si>
+    <t>B13D49</t>
   </si>
 </sst>
 </file>
@@ -404,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +445,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2">
         <v>2019</v>
@@ -451,7 +454,7 @@
         <v>2020</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
@@ -462,7 +465,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>49.331000000000003</v>
+        <v>49.323999999999998</v>
       </c>
       <c r="B3" s="2">
         <v>2019</v>
@@ -474,9 +477,29 @@
         <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>49.325000000000003</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="2">
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2">
         <v>4</v>
       </c>
     </row>

</xml_diff>